<commit_message>
Aggiornamento per nuova pull request
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CARDIONET/CAW04.04.25/accreditamento-checklist_V8.2.6.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CARDIONET/CAW04.04.25/accreditamento-checklist_V8.2.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insiel-my.sharepoint.com/personal/franco_lazzarato_insiel_it/Documents/CDA2_CARDIO/Accreditamento_prima_prova/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\insiel\dati\Divisione Sanità\LB\C@rdionet\ACCREDITAMENTOCDA2\Accreditamento_prima_prova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="544" documentId="13_ncr:1_{7CE019D6-91BC-41F2-9BA1-94B09D0BCFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C54B9EFC-3EA2-496D-B25A-A5DA08ADF4E7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE35CC8-13AD-4D64-8DAB-7EAEFCE39997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="577">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1727,9 +1727,6 @@
   <si>
     <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t>I DATI OPZIONALI RICHIESTI NON SONO GESTITI DALL'APPLICATIVO</t>
   </si>
   <si>
     <t>I dati opzionali richiesti non sono gestiti dall'applicativo</t>
@@ -2882,10 +2879,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4256,10 +4249,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G184" sqref="G184"/>
+      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4308,7 +4301,7 @@
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="51" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D2" s="50"/>
       <c r="F2" s="6"/>
@@ -4739,7 +4732,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="12.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -5047,7 +5040,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="12.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -5279,9 +5272,7 @@
         <v>441</v>
       </c>
       <c r="T28" s="38"/>
-      <c r="U28" s="39" t="s">
-        <v>64</v>
-      </c>
+      <c r="U28" s="39"/>
       <c r="V28" s="40"/>
       <c r="W28" s="38" t="s">
         <v>44</v>
@@ -5365,7 +5356,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="12.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35">
         <v>48</v>
       </c>
@@ -5402,9 +5393,7 @@
       <c r="R31" s="38"/>
       <c r="S31" s="38"/>
       <c r="T31" s="38"/>
-      <c r="U31" s="39" t="s">
-        <v>64</v>
-      </c>
+      <c r="U31" s="39"/>
       <c r="V31" s="40"/>
       <c r="W31" s="38" t="s">
         <v>44</v>
@@ -5864,7 +5853,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>66</v>
       </c>
@@ -5888,7 +5877,7 @@
         <v>228</v>
       </c>
       <c r="K44" s="38" t="s">
-        <v>442</v>
+        <v>233</v>
       </c>
       <c r="L44" s="38"/>
       <c r="M44" s="38"/>
@@ -5922,16 +5911,16 @@
         <v>296</v>
       </c>
       <c r="F45" s="37" t="s">
+        <v>541</v>
+      </c>
+      <c r="G45" s="37" t="s">
         <v>542</v>
       </c>
-      <c r="G45" s="37" t="s">
+      <c r="H45" s="37" t="s">
         <v>543</v>
       </c>
-      <c r="H45" s="37" t="s">
+      <c r="I45" s="42" t="s">
         <v>544</v>
-      </c>
-      <c r="I45" s="42" t="s">
-        <v>545</v>
       </c>
       <c r="J45" s="38" t="s">
         <v>64</v>
@@ -5945,7 +5934,7 @@
         <v>64</v>
       </c>
       <c r="O45" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P45" s="46" t="s">
         <v>64</v>
@@ -5957,7 +5946,7 @@
         <v>228</v>
       </c>
       <c r="S45" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T45" s="38" t="s">
         <v>226</v>
@@ -5985,16 +5974,16 @@
         <v>297</v>
       </c>
       <c r="F46" s="37" t="s">
+        <v>545</v>
+      </c>
+      <c r="G46" s="37" t="s">
         <v>546</v>
       </c>
-      <c r="G46" s="37" t="s">
+      <c r="H46" s="37" t="s">
         <v>547</v>
       </c>
-      <c r="H46" s="37" t="s">
+      <c r="I46" s="42" t="s">
         <v>548</v>
-      </c>
-      <c r="I46" s="42" t="s">
-        <v>549</v>
       </c>
       <c r="J46" s="38" t="s">
         <v>64</v>
@@ -6008,7 +5997,7 @@
         <v>64</v>
       </c>
       <c r="O46" s="38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P46" s="46" t="s">
         <v>64</v>
@@ -6020,7 +6009,7 @@
         <v>228</v>
       </c>
       <c r="S46" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T46" s="38" t="s">
         <v>226</v>
@@ -6048,16 +6037,16 @@
         <v>298</v>
       </c>
       <c r="F47" s="37" t="s">
+        <v>549</v>
+      </c>
+      <c r="G47" s="37" t="s">
         <v>550</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="H47" s="37" t="s">
         <v>551</v>
       </c>
-      <c r="H47" s="37" t="s">
+      <c r="I47" s="42" t="s">
         <v>552</v>
-      </c>
-      <c r="I47" s="42" t="s">
-        <v>553</v>
       </c>
       <c r="J47" s="38" t="s">
         <v>64</v>
@@ -6071,7 +6060,7 @@
         <v>64</v>
       </c>
       <c r="O47" s="38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="P47" s="46" t="s">
         <v>64</v>
@@ -6083,7 +6072,7 @@
         <v>228</v>
       </c>
       <c r="S47" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T47" s="38" t="s">
         <v>226</v>
@@ -6111,16 +6100,16 @@
         <v>299</v>
       </c>
       <c r="F48" s="37" t="s">
+        <v>553</v>
+      </c>
+      <c r="G48" s="37" t="s">
         <v>554</v>
       </c>
-      <c r="G48" s="37" t="s">
+      <c r="H48" s="37" t="s">
         <v>555</v>
       </c>
-      <c r="H48" s="37" t="s">
+      <c r="I48" s="42" t="s">
         <v>556</v>
-      </c>
-      <c r="I48" s="42" t="s">
-        <v>557</v>
       </c>
       <c r="J48" s="38" t="s">
         <v>64</v>
@@ -6134,7 +6123,7 @@
         <v>64</v>
       </c>
       <c r="O48" s="38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P48" s="46" t="s">
         <v>64</v>
@@ -6146,7 +6135,7 @@
         <v>228</v>
       </c>
       <c r="S48" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T48" s="38" t="s">
         <v>226</v>
@@ -6174,16 +6163,16 @@
         <v>300</v>
       </c>
       <c r="F49" s="37" t="s">
+        <v>557</v>
+      </c>
+      <c r="G49" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="H49" s="37" t="s">
         <v>559</v>
       </c>
-      <c r="H49" s="37" t="s">
+      <c r="I49" s="42" t="s">
         <v>560</v>
-      </c>
-      <c r="I49" s="42" t="s">
-        <v>561</v>
       </c>
       <c r="J49" s="38" t="s">
         <v>64</v>
@@ -6197,7 +6186,7 @@
         <v>64</v>
       </c>
       <c r="O49" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P49" s="46" t="s">
         <v>64</v>
@@ -6209,7 +6198,7 @@
         <v>228</v>
       </c>
       <c r="S49" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T49" s="38" t="s">
         <v>226</v>
@@ -6237,16 +6226,16 @@
         <v>301</v>
       </c>
       <c r="F50" s="37" t="s">
+        <v>561</v>
+      </c>
+      <c r="G50" s="37" t="s">
         <v>562</v>
       </c>
-      <c r="G50" s="37" t="s">
+      <c r="H50" s="37" t="s">
         <v>563</v>
       </c>
-      <c r="H50" s="37" t="s">
+      <c r="I50" s="42" t="s">
         <v>564</v>
-      </c>
-      <c r="I50" s="42" t="s">
-        <v>565</v>
       </c>
       <c r="J50" s="38" t="s">
         <v>64</v>
@@ -6260,7 +6249,7 @@
         <v>64</v>
       </c>
       <c r="O50" s="38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P50" s="46" t="s">
         <v>64</v>
@@ -6272,7 +6261,7 @@
         <v>228</v>
       </c>
       <c r="S50" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T50" s="38" t="s">
         <v>226</v>
@@ -6300,16 +6289,16 @@
         <v>302</v>
       </c>
       <c r="F51" s="37" t="s">
+        <v>565</v>
+      </c>
+      <c r="G51" s="37" t="s">
         <v>566</v>
       </c>
-      <c r="G51" s="37" t="s">
+      <c r="H51" s="37" t="s">
         <v>567</v>
       </c>
-      <c r="H51" s="37" t="s">
+      <c r="I51" s="42" t="s">
         <v>568</v>
-      </c>
-      <c r="I51" s="42" t="s">
-        <v>569</v>
       </c>
       <c r="J51" s="38" t="s">
         <v>64</v>
@@ -6323,7 +6312,7 @@
         <v>64</v>
       </c>
       <c r="O51" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P51" s="46" t="s">
         <v>64</v>
@@ -6335,7 +6324,7 @@
         <v>228</v>
       </c>
       <c r="S51" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T51" s="38" t="s">
         <v>226</v>
@@ -6363,16 +6352,16 @@
         <v>303</v>
       </c>
       <c r="F52" s="37" t="s">
+        <v>569</v>
+      </c>
+      <c r="G52" s="37" t="s">
         <v>570</v>
       </c>
-      <c r="G52" s="37" t="s">
+      <c r="H52" s="37" t="s">
         <v>571</v>
       </c>
-      <c r="H52" s="37" t="s">
+      <c r="I52" s="42" t="s">
         <v>572</v>
-      </c>
-      <c r="I52" s="42" t="s">
-        <v>573</v>
       </c>
       <c r="J52" s="38" t="s">
         <v>64</v>
@@ -6386,7 +6375,7 @@
         <v>64</v>
       </c>
       <c r="O52" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P52" s="46" t="s">
         <v>64</v>
@@ -6398,7 +6387,7 @@
         <v>228</v>
       </c>
       <c r="S52" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T52" s="38" t="s">
         <v>226</v>
@@ -8740,7 +8729,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="12.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="35">
         <v>152</v>
       </c>
@@ -8781,7 +8770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="12.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="35">
         <v>154</v>
       </c>
@@ -8805,7 +8794,7 @@
         <v>228</v>
       </c>
       <c r="K117" s="38" t="s">
-        <v>442</v>
+        <v>233</v>
       </c>
       <c r="L117" s="38"/>
       <c r="M117" s="38"/>
@@ -8822,7 +8811,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="35">
         <v>155</v>
       </c>
@@ -8839,16 +8828,16 @@
         <v>341</v>
       </c>
       <c r="F118" s="37" t="s">
+        <v>473</v>
+      </c>
+      <c r="G118" s="37" t="s">
         <v>474</v>
       </c>
-      <c r="G118" s="37" t="s">
+      <c r="H118" s="37" t="s">
         <v>475</v>
       </c>
-      <c r="H118" s="37" t="s">
+      <c r="I118" s="42" t="s">
         <v>476</v>
-      </c>
-      <c r="I118" s="42" t="s">
-        <v>477</v>
       </c>
       <c r="J118" s="38" t="s">
         <v>64</v>
@@ -8862,7 +8851,7 @@
         <v>64</v>
       </c>
       <c r="O118" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P118" s="46" t="s">
         <v>64</v>
@@ -8874,7 +8863,7 @@
         <v>228</v>
       </c>
       <c r="S118" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T118" s="38" t="s">
         <v>226</v>
@@ -8885,7 +8874,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="35">
         <v>156</v>
       </c>
@@ -8902,16 +8891,16 @@
         <v>342</v>
       </c>
       <c r="F119" s="37" t="s">
+        <v>477</v>
+      </c>
+      <c r="G119" s="37" t="s">
         <v>478</v>
       </c>
-      <c r="G119" s="37" t="s">
+      <c r="H119" s="37" t="s">
         <v>479</v>
       </c>
-      <c r="H119" s="37" t="s">
+      <c r="I119" s="42" t="s">
         <v>480</v>
-      </c>
-      <c r="I119" s="42" t="s">
-        <v>481</v>
       </c>
       <c r="J119" s="38" t="s">
         <v>64</v>
@@ -8925,7 +8914,7 @@
         <v>64</v>
       </c>
       <c r="O119" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P119" s="46" t="s">
         <v>64</v>
@@ -8937,7 +8926,7 @@
         <v>228</v>
       </c>
       <c r="S119" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T119" s="38" t="s">
         <v>226</v>
@@ -8948,7 +8937,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="35">
         <v>159</v>
       </c>
@@ -8965,16 +8954,16 @@
         <v>188</v>
       </c>
       <c r="F120" s="37" t="s">
+        <v>481</v>
+      </c>
+      <c r="G120" s="37" t="s">
         <v>482</v>
       </c>
-      <c r="G120" s="37" t="s">
+      <c r="H120" s="37" t="s">
         <v>483</v>
       </c>
-      <c r="H120" s="37" t="s">
+      <c r="I120" s="42" t="s">
         <v>484</v>
-      </c>
-      <c r="I120" s="42" t="s">
-        <v>485</v>
       </c>
       <c r="J120" s="38" t="s">
         <v>64</v>
@@ -8988,7 +8977,7 @@
         <v>64</v>
       </c>
       <c r="O120" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="P120" s="46" t="s">
         <v>64</v>
@@ -9000,7 +8989,7 @@
         <v>228</v>
       </c>
       <c r="S120" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T120" s="38" t="s">
         <v>226</v>
@@ -9011,7 +9000,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="35">
         <v>160</v>
       </c>
@@ -9028,16 +9017,16 @@
         <v>190</v>
       </c>
       <c r="F121" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="G121" s="37" t="s">
         <v>486</v>
       </c>
-      <c r="G121" s="37" t="s">
+      <c r="H121" s="37" t="s">
         <v>487</v>
       </c>
-      <c r="H121" s="37" t="s">
+      <c r="I121" s="42" t="s">
         <v>488</v>
-      </c>
-      <c r="I121" s="42" t="s">
-        <v>489</v>
       </c>
       <c r="J121" s="38" t="s">
         <v>64</v>
@@ -9051,7 +9040,7 @@
         <v>64</v>
       </c>
       <c r="O121" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P121" s="46" t="s">
         <v>64</v>
@@ -9063,7 +9052,7 @@
         <v>228</v>
       </c>
       <c r="S121" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T121" s="38" t="s">
         <v>226</v>
@@ -9074,7 +9063,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="35">
         <v>161</v>
       </c>
@@ -9091,16 +9080,16 @@
         <v>280</v>
       </c>
       <c r="F122" s="37" t="s">
+        <v>489</v>
+      </c>
+      <c r="G122" s="37" t="s">
         <v>490</v>
       </c>
-      <c r="G122" s="37" t="s">
+      <c r="H122" s="37" t="s">
         <v>491</v>
       </c>
-      <c r="H122" s="37" t="s">
+      <c r="I122" s="42" t="s">
         <v>492</v>
-      </c>
-      <c r="I122" s="42" t="s">
-        <v>493</v>
       </c>
       <c r="J122" s="38" t="s">
         <v>64</v>
@@ -9114,7 +9103,7 @@
         <v>64</v>
       </c>
       <c r="O122" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="P122" s="46" t="s">
         <v>64</v>
@@ -9126,7 +9115,7 @@
         <v>228</v>
       </c>
       <c r="S122" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T122" s="38" t="s">
         <v>226</v>
@@ -9137,7 +9126,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="35">
         <v>162</v>
       </c>
@@ -9154,16 +9143,16 @@
         <v>281</v>
       </c>
       <c r="F123" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="G123" s="37" t="s">
         <v>494</v>
       </c>
-      <c r="G123" s="37" t="s">
+      <c r="H123" s="37" t="s">
         <v>495</v>
       </c>
-      <c r="H123" s="37" t="s">
+      <c r="I123" s="42" t="s">
         <v>496</v>
-      </c>
-      <c r="I123" s="42" t="s">
-        <v>497</v>
       </c>
       <c r="J123" s="38" t="s">
         <v>64</v>
@@ -9177,7 +9166,7 @@
         <v>64</v>
       </c>
       <c r="O123" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P123" s="46" t="s">
         <v>64</v>
@@ -9189,7 +9178,7 @@
         <v>228</v>
       </c>
       <c r="S123" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T123" s="38" t="s">
         <v>226</v>
@@ -9200,7 +9189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="35">
         <v>163</v>
       </c>
@@ -9217,16 +9206,16 @@
         <v>282</v>
       </c>
       <c r="F124" s="37" t="s">
+        <v>497</v>
+      </c>
+      <c r="G124" s="37" t="s">
         <v>498</v>
       </c>
-      <c r="G124" s="37" t="s">
+      <c r="H124" s="37" t="s">
         <v>499</v>
       </c>
-      <c r="H124" s="37" t="s">
+      <c r="I124" s="42" t="s">
         <v>500</v>
-      </c>
-      <c r="I124" s="42" t="s">
-        <v>501</v>
       </c>
       <c r="J124" s="38" t="s">
         <v>64</v>
@@ -9240,7 +9229,7 @@
         <v>64</v>
       </c>
       <c r="O124" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P124" s="46" t="s">
         <v>64</v>
@@ -9252,7 +9241,7 @@
         <v>228</v>
       </c>
       <c r="S124" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T124" s="38" t="s">
         <v>226</v>
@@ -9263,7 +9252,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="35">
         <v>164</v>
       </c>
@@ -9280,16 +9269,16 @@
         <v>283</v>
       </c>
       <c r="F125" s="37" t="s">
+        <v>501</v>
+      </c>
+      <c r="G125" s="37" t="s">
         <v>502</v>
       </c>
-      <c r="G125" s="37" t="s">
+      <c r="H125" s="37" t="s">
         <v>503</v>
       </c>
-      <c r="H125" s="37" t="s">
+      <c r="I125" s="42" t="s">
         <v>504</v>
-      </c>
-      <c r="I125" s="42" t="s">
-        <v>505</v>
       </c>
       <c r="J125" s="38" t="s">
         <v>64</v>
@@ -9303,7 +9292,7 @@
         <v>64</v>
       </c>
       <c r="O125" s="38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P125" s="46" t="s">
         <v>64</v>
@@ -9315,7 +9304,7 @@
         <v>228</v>
       </c>
       <c r="S125" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T125" s="38" t="s">
         <v>226</v>
@@ -9326,7 +9315,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="35">
         <v>165</v>
       </c>
@@ -9343,16 +9332,16 @@
         <v>284</v>
       </c>
       <c r="F126" s="37" t="s">
+        <v>505</v>
+      </c>
+      <c r="G126" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="G126" s="37" t="s">
+      <c r="H126" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="H126" s="37" t="s">
+      <c r="I126" s="42" t="s">
         <v>508</v>
-      </c>
-      <c r="I126" s="42" t="s">
-        <v>509</v>
       </c>
       <c r="J126" s="38" t="s">
         <v>64</v>
@@ -9366,7 +9355,7 @@
         <v>64</v>
       </c>
       <c r="O126" s="38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="P126" s="46" t="s">
         <v>64</v>
@@ -9378,7 +9367,7 @@
         <v>228</v>
       </c>
       <c r="S126" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T126" s="38" t="s">
         <v>226</v>
@@ -9389,7 +9378,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="35">
         <v>166</v>
       </c>
@@ -9406,16 +9395,16 @@
         <v>285</v>
       </c>
       <c r="F127" s="37" t="s">
+        <v>509</v>
+      </c>
+      <c r="G127" s="37" t="s">
         <v>510</v>
       </c>
-      <c r="G127" s="37" t="s">
+      <c r="H127" s="37" t="s">
         <v>511</v>
       </c>
-      <c r="H127" s="37" t="s">
+      <c r="I127" s="42" t="s">
         <v>512</v>
-      </c>
-      <c r="I127" s="42" t="s">
-        <v>513</v>
       </c>
       <c r="J127" s="38" t="s">
         <v>64</v>
@@ -9429,7 +9418,7 @@
         <v>64</v>
       </c>
       <c r="O127" s="38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P127" s="46" t="s">
         <v>64</v>
@@ -9441,7 +9430,7 @@
         <v>228</v>
       </c>
       <c r="S127" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T127" s="38" t="s">
         <v>226</v>
@@ -9452,7 +9441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="35">
         <v>167</v>
       </c>
@@ -9469,16 +9458,16 @@
         <v>286</v>
       </c>
       <c r="F128" s="37" t="s">
+        <v>513</v>
+      </c>
+      <c r="G128" s="37" t="s">
         <v>514</v>
       </c>
-      <c r="G128" s="37" t="s">
+      <c r="H128" s="37" t="s">
         <v>515</v>
       </c>
-      <c r="H128" s="37" t="s">
+      <c r="I128" s="42" t="s">
         <v>516</v>
-      </c>
-      <c r="I128" s="42" t="s">
-        <v>517</v>
       </c>
       <c r="J128" s="38" t="s">
         <v>64</v>
@@ -9492,7 +9481,7 @@
         <v>64</v>
       </c>
       <c r="O128" s="38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P128" s="46" t="s">
         <v>64</v>
@@ -9504,7 +9493,7 @@
         <v>228</v>
       </c>
       <c r="S128" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T128" s="38" t="s">
         <v>226</v>
@@ -9515,7 +9504,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="35">
         <v>168</v>
       </c>
@@ -9532,16 +9521,16 @@
         <v>287</v>
       </c>
       <c r="F129" s="37" t="s">
+        <v>517</v>
+      </c>
+      <c r="G129" s="37" t="s">
         <v>518</v>
       </c>
-      <c r="G129" s="37" t="s">
+      <c r="H129" s="37" t="s">
         <v>519</v>
       </c>
-      <c r="H129" s="37" t="s">
+      <c r="I129" s="42" t="s">
         <v>520</v>
-      </c>
-      <c r="I129" s="42" t="s">
-        <v>521</v>
       </c>
       <c r="J129" s="38" t="s">
         <v>64</v>
@@ -9555,7 +9544,7 @@
         <v>64</v>
       </c>
       <c r="O129" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="P129" s="46" t="s">
         <v>64</v>
@@ -9567,7 +9556,7 @@
         <v>228</v>
       </c>
       <c r="S129" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T129" s="38" t="s">
         <v>226</v>
@@ -9578,7 +9567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="35">
         <v>169</v>
       </c>
@@ -9595,16 +9584,16 @@
         <v>289</v>
       </c>
       <c r="F130" s="37" t="s">
+        <v>521</v>
+      </c>
+      <c r="G130" s="37" t="s">
         <v>522</v>
       </c>
-      <c r="G130" s="37" t="s">
+      <c r="H130" s="37" t="s">
         <v>523</v>
       </c>
-      <c r="H130" s="37" t="s">
+      <c r="I130" s="42" t="s">
         <v>524</v>
-      </c>
-      <c r="I130" s="42" t="s">
-        <v>525</v>
       </c>
       <c r="J130" s="38" t="s">
         <v>64</v>
@@ -9618,7 +9607,7 @@
         <v>64</v>
       </c>
       <c r="O130" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="P130" s="46" t="s">
         <v>64</v>
@@ -9630,7 +9619,7 @@
         <v>228</v>
       </c>
       <c r="S130" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T130" s="38" t="s">
         <v>226</v>
@@ -10936,7 +10925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="35">
         <v>448</v>
       </c>
@@ -10953,16 +10942,16 @@
         <v>389</v>
       </c>
       <c r="F166" s="37" t="s">
+        <v>469</v>
+      </c>
+      <c r="G166" s="37" t="s">
         <v>470</v>
       </c>
-      <c r="G166" s="37" t="s">
+      <c r="H166" s="37" t="s">
         <v>471</v>
       </c>
-      <c r="H166" s="37" t="s">
+      <c r="I166" s="42" t="s">
         <v>472</v>
-      </c>
-      <c r="I166" s="42" t="s">
-        <v>473</v>
       </c>
       <c r="J166" s="38" t="s">
         <v>64</v>
@@ -10985,7 +10974,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="12.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="35">
         <v>449</v>
       </c>
@@ -11012,7 +11001,7 @@
         <v>239</v>
       </c>
       <c r="L167" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M167" s="38"/>
       <c r="N167" s="38"/>
@@ -11045,16 +11034,16 @@
         <v>373</v>
       </c>
       <c r="F168" s="37" t="s">
+        <v>537</v>
+      </c>
+      <c r="G168" s="37" t="s">
         <v>538</v>
       </c>
-      <c r="G168" s="37" t="s">
+      <c r="H168" s="37" t="s">
         <v>539</v>
       </c>
-      <c r="H168" s="37" t="s">
+      <c r="I168" s="42" t="s">
         <v>540</v>
-      </c>
-      <c r="I168" s="42" t="s">
-        <v>541</v>
       </c>
       <c r="J168" s="38" t="s">
         <v>64</v>
@@ -11077,7 +11066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="35">
         <v>451</v>
       </c>
@@ -11101,7 +11090,7 @@
         <v>228</v>
       </c>
       <c r="K169" s="38" t="s">
-        <v>442</v>
+        <v>233</v>
       </c>
       <c r="L169" s="38"/>
       <c r="M169" s="38"/>
@@ -11414,7 +11403,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="35">
         <v>461</v>
       </c>
@@ -11431,16 +11420,16 @@
         <v>391</v>
       </c>
       <c r="F178" s="35" t="s">
+        <v>525</v>
+      </c>
+      <c r="G178" s="37" t="s">
         <v>526</v>
       </c>
-      <c r="G178" s="37" t="s">
+      <c r="H178" s="35" t="s">
         <v>527</v>
       </c>
-      <c r="H178" s="35" t="s">
+      <c r="I178" s="42" t="s">
         <v>528</v>
-      </c>
-      <c r="I178" s="42" t="s">
-        <v>529</v>
       </c>
       <c r="J178" s="38" t="s">
         <v>64</v>
@@ -11454,7 +11443,7 @@
         <v>64</v>
       </c>
       <c r="O178" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P178" s="38" t="s">
         <v>64</v>
@@ -11466,7 +11455,7 @@
         <v>228</v>
       </c>
       <c r="S178" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T178" s="38" t="s">
         <v>226</v>
@@ -11679,16 +11668,16 @@
         <v>404</v>
       </c>
       <c r="F184" s="35" t="s">
+        <v>573</v>
+      </c>
+      <c r="G184" s="37" t="s">
         <v>574</v>
       </c>
-      <c r="G184" s="37" t="s">
+      <c r="H184" s="35" t="s">
         <v>575</v>
       </c>
-      <c r="H184" s="35" t="s">
+      <c r="I184" s="42" t="s">
         <v>576</v>
-      </c>
-      <c r="I184" s="42" t="s">
-        <v>577</v>
       </c>
       <c r="J184" s="38" t="s">
         <v>64</v>
@@ -11702,7 +11691,7 @@
         <v>64</v>
       </c>
       <c r="O184" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P184" s="46" t="s">
         <v>64</v>
@@ -11714,7 +11703,7 @@
         <v>228</v>
       </c>
       <c r="S184" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T184" s="38" t="s">
         <v>226</v>
@@ -11725,7 +11714,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="35">
         <v>468</v>
       </c>
@@ -11742,16 +11731,16 @@
         <v>406</v>
       </c>
       <c r="F185" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="G185" s="37" t="s">
         <v>530</v>
       </c>
-      <c r="G185" s="37" t="s">
+      <c r="H185" s="35" t="s">
         <v>531</v>
       </c>
-      <c r="H185" s="35" t="s">
+      <c r="I185" s="42" t="s">
         <v>532</v>
-      </c>
-      <c r="I185" s="42" t="s">
-        <v>533</v>
       </c>
       <c r="J185" s="38" t="s">
         <v>64</v>
@@ -11765,7 +11754,7 @@
         <v>64</v>
       </c>
       <c r="O185" s="38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P185" s="38" t="s">
         <v>64</v>
@@ -11777,7 +11766,7 @@
         <v>228</v>
       </c>
       <c r="S185" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T185" s="38" t="s">
         <v>226</v>
@@ -12010,7 +11999,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="35">
         <v>475</v>
       </c>
@@ -12027,16 +12016,16 @@
         <v>433</v>
       </c>
       <c r="F192" s="37" t="s">
+        <v>533</v>
+      </c>
+      <c r="G192" s="37" t="s">
         <v>534</v>
       </c>
-      <c r="G192" s="37" t="s">
+      <c r="H192" s="37" t="s">
         <v>535</v>
       </c>
-      <c r="H192" s="37" t="s">
+      <c r="I192" s="42" t="s">
         <v>536</v>
-      </c>
-      <c r="I192" s="42" t="s">
-        <v>537</v>
       </c>
       <c r="J192" s="38" t="s">
         <v>64</v>
@@ -12050,7 +12039,7 @@
         <v>64</v>
       </c>
       <c r="O192" s="38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P192" s="38" t="s">
         <v>64</v>
@@ -12062,7 +12051,7 @@
         <v>228</v>
       </c>
       <c r="S192" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T192" s="38" t="s">
         <v>226</v>
@@ -16094,6 +16083,7 @@
     <filterColumn colId="2">
       <filters>
         <filter val="LDO"/>
+        <filter val="RSA"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -18380,12 +18370,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b6c6c545-4433-4453-a388-ae81a1a09069" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ae8219d-8505-4e64-b47a-e5e02bd99ff8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18612,29 +18604,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b6c6c545-4433-4453-a388-ae81a1a09069" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ae8219d-8505-4e64-b47a-e5e02bd99ff8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25F1C044-501F-4A34-A6FC-55ED2C028642}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -18651,6 +18629,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD34699-60E0-49C2-BE80-D215B28F2689}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
commit accreditamento-checklist_V8.2.6.xlsx per aggiornamento pull request
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CARDIONET/CAW04.04.25/accreditamento-checklist_V8.2.6.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CARDIONET/CAW04.04.25/accreditamento-checklist_V8.2.6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\insiel\dati\Divisione Sanità\LB\C@rdionet\ACCREDITAMENTOCDA2\Accreditamento_prima_prova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE35CC8-13AD-4D64-8DAB-7EAEFCE39997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8297662A-6226-4BCE-8F22-FD89165670DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="578">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1725,10 +1725,6 @@
     <t>TEST NON ESEGUIBILE PERCHE' SARA' OGGETTO DELL'ACCREDITAMENTO DEL MIDDLEWARE REGIONALE</t>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
     <t>I dati opzionali richiesti non sono gestiti dall'applicativo</t>
   </si>
   <si>
@@ -2156,6 +2152,13 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.60.4.4.be4aeef218c47ad36ca74dbc00040a21f1cfd38836a7a712039f17f6de45bc0f.5eb81f2977^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I MESSAGGI ANDATI IN ERRORE VENGONO PERIODICAMENTE RIPROCESSATI
+</t>
+  </si>
+  <si>
+    <t>I MESSAGGI ANDATI IN ERRORE VENGONO PERIODICAMENTE RIPROCESSATI</t>
   </si>
 </sst>
 </file>
@@ -4249,10 +4252,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="L12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomRight" activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4301,7 +4304,7 @@
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="51" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D2" s="50"/>
       <c r="F2" s="6"/>
@@ -5256,20 +5259,26 @@
       <c r="J28" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K28" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="L28" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N28" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O28" s="38"/>
-      <c r="P28" s="38"/>
-      <c r="Q28" s="38"/>
-      <c r="R28" s="38"/>
+      <c r="P28" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q28" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R28" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="S28" s="38" t="s">
-        <v>441</v>
+        <v>576</v>
       </c>
       <c r="T28" s="38"/>
       <c r="U28" s="39"/>
@@ -5379,19 +5388,27 @@
       <c r="J31" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K31" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="L31" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="M31" s="38"/>
-      <c r="N31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N31" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O31" s="38"/>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="38"/>
-      <c r="R31" s="38"/>
-      <c r="S31" s="38"/>
+      <c r="P31" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q31" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R31" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S31" s="38" t="s">
+        <v>577</v>
+      </c>
       <c r="T31" s="38"/>
       <c r="U31" s="39"/>
       <c r="V31" s="40"/>
@@ -5911,16 +5928,16 @@
         <v>296</v>
       </c>
       <c r="F45" s="37" t="s">
+        <v>540</v>
+      </c>
+      <c r="G45" s="37" t="s">
         <v>541</v>
       </c>
-      <c r="G45" s="37" t="s">
+      <c r="H45" s="37" t="s">
         <v>542</v>
       </c>
-      <c r="H45" s="37" t="s">
+      <c r="I45" s="42" t="s">
         <v>543</v>
-      </c>
-      <c r="I45" s="42" t="s">
-        <v>544</v>
       </c>
       <c r="J45" s="38" t="s">
         <v>64</v>
@@ -5934,7 +5951,7 @@
         <v>64</v>
       </c>
       <c r="O45" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P45" s="46" t="s">
         <v>64</v>
@@ -5946,7 +5963,7 @@
         <v>228</v>
       </c>
       <c r="S45" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T45" s="38" t="s">
         <v>226</v>
@@ -5974,16 +5991,16 @@
         <v>297</v>
       </c>
       <c r="F46" s="37" t="s">
+        <v>544</v>
+      </c>
+      <c r="G46" s="37" t="s">
         <v>545</v>
       </c>
-      <c r="G46" s="37" t="s">
+      <c r="H46" s="37" t="s">
         <v>546</v>
       </c>
-      <c r="H46" s="37" t="s">
+      <c r="I46" s="42" t="s">
         <v>547</v>
-      </c>
-      <c r="I46" s="42" t="s">
-        <v>548</v>
       </c>
       <c r="J46" s="38" t="s">
         <v>64</v>
@@ -5997,7 +6014,7 @@
         <v>64</v>
       </c>
       <c r="O46" s="38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P46" s="46" t="s">
         <v>64</v>
@@ -6009,7 +6026,7 @@
         <v>228</v>
       </c>
       <c r="S46" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T46" s="38" t="s">
         <v>226</v>
@@ -6037,16 +6054,16 @@
         <v>298</v>
       </c>
       <c r="F47" s="37" t="s">
+        <v>548</v>
+      </c>
+      <c r="G47" s="37" t="s">
         <v>549</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="H47" s="37" t="s">
         <v>550</v>
       </c>
-      <c r="H47" s="37" t="s">
+      <c r="I47" s="42" t="s">
         <v>551</v>
-      </c>
-      <c r="I47" s="42" t="s">
-        <v>552</v>
       </c>
       <c r="J47" s="38" t="s">
         <v>64</v>
@@ -6060,7 +6077,7 @@
         <v>64</v>
       </c>
       <c r="O47" s="38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P47" s="46" t="s">
         <v>64</v>
@@ -6072,7 +6089,7 @@
         <v>228</v>
       </c>
       <c r="S47" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T47" s="38" t="s">
         <v>226</v>
@@ -6100,16 +6117,16 @@
         <v>299</v>
       </c>
       <c r="F48" s="37" t="s">
+        <v>552</v>
+      </c>
+      <c r="G48" s="37" t="s">
         <v>553</v>
       </c>
-      <c r="G48" s="37" t="s">
+      <c r="H48" s="37" t="s">
         <v>554</v>
       </c>
-      <c r="H48" s="37" t="s">
+      <c r="I48" s="42" t="s">
         <v>555</v>
-      </c>
-      <c r="I48" s="42" t="s">
-        <v>556</v>
       </c>
       <c r="J48" s="38" t="s">
         <v>64</v>
@@ -6123,7 +6140,7 @@
         <v>64</v>
       </c>
       <c r="O48" s="38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="P48" s="46" t="s">
         <v>64</v>
@@ -6135,7 +6152,7 @@
         <v>228</v>
       </c>
       <c r="S48" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T48" s="38" t="s">
         <v>226</v>
@@ -6163,16 +6180,16 @@
         <v>300</v>
       </c>
       <c r="F49" s="37" t="s">
+        <v>556</v>
+      </c>
+      <c r="G49" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="H49" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="H49" s="37" t="s">
+      <c r="I49" s="42" t="s">
         <v>559</v>
-      </c>
-      <c r="I49" s="42" t="s">
-        <v>560</v>
       </c>
       <c r="J49" s="38" t="s">
         <v>64</v>
@@ -6186,7 +6203,7 @@
         <v>64</v>
       </c>
       <c r="O49" s="38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P49" s="46" t="s">
         <v>64</v>
@@ -6198,7 +6215,7 @@
         <v>228</v>
       </c>
       <c r="S49" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T49" s="38" t="s">
         <v>226</v>
@@ -6226,16 +6243,16 @@
         <v>301</v>
       </c>
       <c r="F50" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="G50" s="37" t="s">
         <v>561</v>
       </c>
-      <c r="G50" s="37" t="s">
+      <c r="H50" s="37" t="s">
         <v>562</v>
       </c>
-      <c r="H50" s="37" t="s">
+      <c r="I50" s="42" t="s">
         <v>563</v>
-      </c>
-      <c r="I50" s="42" t="s">
-        <v>564</v>
       </c>
       <c r="J50" s="38" t="s">
         <v>64</v>
@@ -6249,7 +6266,7 @@
         <v>64</v>
       </c>
       <c r="O50" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P50" s="46" t="s">
         <v>64</v>
@@ -6261,7 +6278,7 @@
         <v>228</v>
       </c>
       <c r="S50" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T50" s="38" t="s">
         <v>226</v>
@@ -6289,16 +6306,16 @@
         <v>302</v>
       </c>
       <c r="F51" s="37" t="s">
+        <v>564</v>
+      </c>
+      <c r="G51" s="37" t="s">
         <v>565</v>
       </c>
-      <c r="G51" s="37" t="s">
+      <c r="H51" s="37" t="s">
         <v>566</v>
       </c>
-      <c r="H51" s="37" t="s">
+      <c r="I51" s="42" t="s">
         <v>567</v>
-      </c>
-      <c r="I51" s="42" t="s">
-        <v>568</v>
       </c>
       <c r="J51" s="38" t="s">
         <v>64</v>
@@ -6312,7 +6329,7 @@
         <v>64</v>
       </c>
       <c r="O51" s="38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P51" s="46" t="s">
         <v>64</v>
@@ -6324,7 +6341,7 @@
         <v>228</v>
       </c>
       <c r="S51" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T51" s="38" t="s">
         <v>226</v>
@@ -6352,16 +6369,16 @@
         <v>303</v>
       </c>
       <c r="F52" s="37" t="s">
+        <v>568</v>
+      </c>
+      <c r="G52" s="37" t="s">
         <v>569</v>
       </c>
-      <c r="G52" s="37" t="s">
+      <c r="H52" s="37" t="s">
         <v>570</v>
       </c>
-      <c r="H52" s="37" t="s">
+      <c r="I52" s="42" t="s">
         <v>571</v>
-      </c>
-      <c r="I52" s="42" t="s">
-        <v>572</v>
       </c>
       <c r="J52" s="38" t="s">
         <v>64</v>
@@ -6375,7 +6392,7 @@
         <v>64</v>
       </c>
       <c r="O52" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P52" s="46" t="s">
         <v>64</v>
@@ -6387,7 +6404,7 @@
         <v>228</v>
       </c>
       <c r="S52" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T52" s="38" t="s">
         <v>226</v>
@@ -8828,16 +8845,16 @@
         <v>341</v>
       </c>
       <c r="F118" s="37" t="s">
+        <v>472</v>
+      </c>
+      <c r="G118" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="G118" s="37" t="s">
+      <c r="H118" s="37" t="s">
         <v>474</v>
       </c>
-      <c r="H118" s="37" t="s">
+      <c r="I118" s="42" t="s">
         <v>475</v>
-      </c>
-      <c r="I118" s="42" t="s">
-        <v>476</v>
       </c>
       <c r="J118" s="38" t="s">
         <v>64</v>
@@ -8851,7 +8868,7 @@
         <v>64</v>
       </c>
       <c r="O118" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P118" s="46" t="s">
         <v>64</v>
@@ -8863,7 +8880,7 @@
         <v>228</v>
       </c>
       <c r="S118" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T118" s="38" t="s">
         <v>226</v>
@@ -8891,16 +8908,16 @@
         <v>342</v>
       </c>
       <c r="F119" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="G119" s="37" t="s">
         <v>477</v>
       </c>
-      <c r="G119" s="37" t="s">
+      <c r="H119" s="37" t="s">
         <v>478</v>
       </c>
-      <c r="H119" s="37" t="s">
+      <c r="I119" s="42" t="s">
         <v>479</v>
-      </c>
-      <c r="I119" s="42" t="s">
-        <v>480</v>
       </c>
       <c r="J119" s="38" t="s">
         <v>64</v>
@@ -8914,7 +8931,7 @@
         <v>64</v>
       </c>
       <c r="O119" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="P119" s="46" t="s">
         <v>64</v>
@@ -8926,7 +8943,7 @@
         <v>228</v>
       </c>
       <c r="S119" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T119" s="38" t="s">
         <v>226</v>
@@ -8954,16 +8971,16 @@
         <v>188</v>
       </c>
       <c r="F120" s="37" t="s">
+        <v>480</v>
+      </c>
+      <c r="G120" s="37" t="s">
         <v>481</v>
       </c>
-      <c r="G120" s="37" t="s">
+      <c r="H120" s="37" t="s">
         <v>482</v>
       </c>
-      <c r="H120" s="37" t="s">
+      <c r="I120" s="42" t="s">
         <v>483</v>
-      </c>
-      <c r="I120" s="42" t="s">
-        <v>484</v>
       </c>
       <c r="J120" s="38" t="s">
         <v>64</v>
@@ -8977,7 +8994,7 @@
         <v>64</v>
       </c>
       <c r="O120" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P120" s="46" t="s">
         <v>64</v>
@@ -8989,7 +9006,7 @@
         <v>228</v>
       </c>
       <c r="S120" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T120" s="38" t="s">
         <v>226</v>
@@ -9017,16 +9034,16 @@
         <v>190</v>
       </c>
       <c r="F121" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="G121" s="37" t="s">
         <v>485</v>
       </c>
-      <c r="G121" s="37" t="s">
+      <c r="H121" s="37" t="s">
         <v>486</v>
       </c>
-      <c r="H121" s="37" t="s">
+      <c r="I121" s="42" t="s">
         <v>487</v>
-      </c>
-      <c r="I121" s="42" t="s">
-        <v>488</v>
       </c>
       <c r="J121" s="38" t="s">
         <v>64</v>
@@ -9040,7 +9057,7 @@
         <v>64</v>
       </c>
       <c r="O121" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P121" s="46" t="s">
         <v>64</v>
@@ -9052,7 +9069,7 @@
         <v>228</v>
       </c>
       <c r="S121" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T121" s="38" t="s">
         <v>226</v>
@@ -9080,16 +9097,16 @@
         <v>280</v>
       </c>
       <c r="F122" s="37" t="s">
+        <v>488</v>
+      </c>
+      <c r="G122" s="37" t="s">
         <v>489</v>
       </c>
-      <c r="G122" s="37" t="s">
+      <c r="H122" s="37" t="s">
         <v>490</v>
       </c>
-      <c r="H122" s="37" t="s">
+      <c r="I122" s="42" t="s">
         <v>491</v>
-      </c>
-      <c r="I122" s="42" t="s">
-        <v>492</v>
       </c>
       <c r="J122" s="38" t="s">
         <v>64</v>
@@ -9103,7 +9120,7 @@
         <v>64</v>
       </c>
       <c r="O122" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P122" s="46" t="s">
         <v>64</v>
@@ -9115,7 +9132,7 @@
         <v>228</v>
       </c>
       <c r="S122" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T122" s="38" t="s">
         <v>226</v>
@@ -9143,16 +9160,16 @@
         <v>281</v>
       </c>
       <c r="F123" s="37" t="s">
+        <v>492</v>
+      </c>
+      <c r="G123" s="37" t="s">
         <v>493</v>
       </c>
-      <c r="G123" s="37" t="s">
+      <c r="H123" s="37" t="s">
         <v>494</v>
       </c>
-      <c r="H123" s="37" t="s">
+      <c r="I123" s="42" t="s">
         <v>495</v>
-      </c>
-      <c r="I123" s="42" t="s">
-        <v>496</v>
       </c>
       <c r="J123" s="38" t="s">
         <v>64</v>
@@ -9166,7 +9183,7 @@
         <v>64</v>
       </c>
       <c r="O123" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="P123" s="46" t="s">
         <v>64</v>
@@ -9178,7 +9195,7 @@
         <v>228</v>
       </c>
       <c r="S123" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T123" s="38" t="s">
         <v>226</v>
@@ -9206,16 +9223,16 @@
         <v>282</v>
       </c>
       <c r="F124" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="G124" s="37" t="s">
         <v>497</v>
       </c>
-      <c r="G124" s="37" t="s">
+      <c r="H124" s="37" t="s">
         <v>498</v>
       </c>
-      <c r="H124" s="37" t="s">
+      <c r="I124" s="42" t="s">
         <v>499</v>
-      </c>
-      <c r="I124" s="42" t="s">
-        <v>500</v>
       </c>
       <c r="J124" s="38" t="s">
         <v>64</v>
@@ -9229,7 +9246,7 @@
         <v>64</v>
       </c>
       <c r="O124" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P124" s="46" t="s">
         <v>64</v>
@@ -9241,7 +9258,7 @@
         <v>228</v>
       </c>
       <c r="S124" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T124" s="38" t="s">
         <v>226</v>
@@ -9269,16 +9286,16 @@
         <v>283</v>
       </c>
       <c r="F125" s="37" t="s">
+        <v>500</v>
+      </c>
+      <c r="G125" s="37" t="s">
         <v>501</v>
       </c>
-      <c r="G125" s="37" t="s">
+      <c r="H125" s="37" t="s">
         <v>502</v>
       </c>
-      <c r="H125" s="37" t="s">
+      <c r="I125" s="42" t="s">
         <v>503</v>
-      </c>
-      <c r="I125" s="42" t="s">
-        <v>504</v>
       </c>
       <c r="J125" s="38" t="s">
         <v>64</v>
@@ -9292,7 +9309,7 @@
         <v>64</v>
       </c>
       <c r="O125" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P125" s="46" t="s">
         <v>64</v>
@@ -9304,7 +9321,7 @@
         <v>228</v>
       </c>
       <c r="S125" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T125" s="38" t="s">
         <v>226</v>
@@ -9332,16 +9349,16 @@
         <v>284</v>
       </c>
       <c r="F126" s="37" t="s">
+        <v>504</v>
+      </c>
+      <c r="G126" s="37" t="s">
         <v>505</v>
       </c>
-      <c r="G126" s="37" t="s">
+      <c r="H126" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="H126" s="37" t="s">
+      <c r="I126" s="42" t="s">
         <v>507</v>
-      </c>
-      <c r="I126" s="42" t="s">
-        <v>508</v>
       </c>
       <c r="J126" s="38" t="s">
         <v>64</v>
@@ -9355,7 +9372,7 @@
         <v>64</v>
       </c>
       <c r="O126" s="38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P126" s="46" t="s">
         <v>64</v>
@@ -9367,7 +9384,7 @@
         <v>228</v>
       </c>
       <c r="S126" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T126" s="38" t="s">
         <v>226</v>
@@ -9395,16 +9412,16 @@
         <v>285</v>
       </c>
       <c r="F127" s="37" t="s">
+        <v>508</v>
+      </c>
+      <c r="G127" s="37" t="s">
         <v>509</v>
       </c>
-      <c r="G127" s="37" t="s">
+      <c r="H127" s="37" t="s">
         <v>510</v>
       </c>
-      <c r="H127" s="37" t="s">
+      <c r="I127" s="42" t="s">
         <v>511</v>
-      </c>
-      <c r="I127" s="42" t="s">
-        <v>512</v>
       </c>
       <c r="J127" s="38" t="s">
         <v>64</v>
@@ -9418,7 +9435,7 @@
         <v>64</v>
       </c>
       <c r="O127" s="38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="P127" s="46" t="s">
         <v>64</v>
@@ -9430,7 +9447,7 @@
         <v>228</v>
       </c>
       <c r="S127" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T127" s="38" t="s">
         <v>226</v>
@@ -9458,16 +9475,16 @@
         <v>286</v>
       </c>
       <c r="F128" s="37" t="s">
+        <v>512</v>
+      </c>
+      <c r="G128" s="37" t="s">
         <v>513</v>
       </c>
-      <c r="G128" s="37" t="s">
+      <c r="H128" s="37" t="s">
         <v>514</v>
       </c>
-      <c r="H128" s="37" t="s">
+      <c r="I128" s="42" t="s">
         <v>515</v>
-      </c>
-      <c r="I128" s="42" t="s">
-        <v>516</v>
       </c>
       <c r="J128" s="38" t="s">
         <v>64</v>
@@ -9481,7 +9498,7 @@
         <v>64</v>
       </c>
       <c r="O128" s="38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P128" s="46" t="s">
         <v>64</v>
@@ -9493,7 +9510,7 @@
         <v>228</v>
       </c>
       <c r="S128" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T128" s="38" t="s">
         <v>226</v>
@@ -9521,16 +9538,16 @@
         <v>287</v>
       </c>
       <c r="F129" s="37" t="s">
+        <v>516</v>
+      </c>
+      <c r="G129" s="37" t="s">
         <v>517</v>
       </c>
-      <c r="G129" s="37" t="s">
+      <c r="H129" s="37" t="s">
         <v>518</v>
       </c>
-      <c r="H129" s="37" t="s">
+      <c r="I129" s="42" t="s">
         <v>519</v>
-      </c>
-      <c r="I129" s="42" t="s">
-        <v>520</v>
       </c>
       <c r="J129" s="38" t="s">
         <v>64</v>
@@ -9544,7 +9561,7 @@
         <v>64</v>
       </c>
       <c r="O129" s="38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P129" s="46" t="s">
         <v>64</v>
@@ -9556,7 +9573,7 @@
         <v>228</v>
       </c>
       <c r="S129" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T129" s="38" t="s">
         <v>226</v>
@@ -9584,16 +9601,16 @@
         <v>289</v>
       </c>
       <c r="F130" s="37" t="s">
+        <v>520</v>
+      </c>
+      <c r="G130" s="37" t="s">
         <v>521</v>
       </c>
-      <c r="G130" s="37" t="s">
+      <c r="H130" s="37" t="s">
         <v>522</v>
       </c>
-      <c r="H130" s="37" t="s">
+      <c r="I130" s="42" t="s">
         <v>523</v>
-      </c>
-      <c r="I130" s="42" t="s">
-        <v>524</v>
       </c>
       <c r="J130" s="38" t="s">
         <v>64</v>
@@ -9607,7 +9624,7 @@
         <v>64</v>
       </c>
       <c r="O130" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="P130" s="46" t="s">
         <v>64</v>
@@ -9619,7 +9636,7 @@
         <v>228</v>
       </c>
       <c r="S130" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T130" s="38" t="s">
         <v>226</v>
@@ -10942,16 +10959,16 @@
         <v>389</v>
       </c>
       <c r="F166" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="G166" s="37" t="s">
         <v>469</v>
       </c>
-      <c r="G166" s="37" t="s">
+      <c r="H166" s="37" t="s">
         <v>470</v>
       </c>
-      <c r="H166" s="37" t="s">
+      <c r="I166" s="42" t="s">
         <v>471</v>
-      </c>
-      <c r="I166" s="42" t="s">
-        <v>472</v>
       </c>
       <c r="J166" s="38" t="s">
         <v>64</v>
@@ -11001,7 +11018,7 @@
         <v>239</v>
       </c>
       <c r="L167" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M167" s="38"/>
       <c r="N167" s="38"/>
@@ -11034,16 +11051,16 @@
         <v>373</v>
       </c>
       <c r="F168" s="37" t="s">
+        <v>536</v>
+      </c>
+      <c r="G168" s="37" t="s">
         <v>537</v>
       </c>
-      <c r="G168" s="37" t="s">
+      <c r="H168" s="37" t="s">
         <v>538</v>
       </c>
-      <c r="H168" s="37" t="s">
+      <c r="I168" s="42" t="s">
         <v>539</v>
-      </c>
-      <c r="I168" s="42" t="s">
-        <v>540</v>
       </c>
       <c r="J168" s="38" t="s">
         <v>64</v>
@@ -11420,16 +11437,16 @@
         <v>391</v>
       </c>
       <c r="F178" s="35" t="s">
+        <v>524</v>
+      </c>
+      <c r="G178" s="37" t="s">
         <v>525</v>
       </c>
-      <c r="G178" s="37" t="s">
+      <c r="H178" s="35" t="s">
         <v>526</v>
       </c>
-      <c r="H178" s="35" t="s">
+      <c r="I178" s="42" t="s">
         <v>527</v>
-      </c>
-      <c r="I178" s="42" t="s">
-        <v>528</v>
       </c>
       <c r="J178" s="38" t="s">
         <v>64</v>
@@ -11443,7 +11460,7 @@
         <v>64</v>
       </c>
       <c r="O178" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="P178" s="38" t="s">
         <v>64</v>
@@ -11455,7 +11472,7 @@
         <v>228</v>
       </c>
       <c r="S178" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T178" s="38" t="s">
         <v>226</v>
@@ -11668,16 +11685,16 @@
         <v>404</v>
       </c>
       <c r="F184" s="35" t="s">
+        <v>572</v>
+      </c>
+      <c r="G184" s="37" t="s">
         <v>573</v>
       </c>
-      <c r="G184" s="37" t="s">
+      <c r="H184" s="35" t="s">
         <v>574</v>
       </c>
-      <c r="H184" s="35" t="s">
+      <c r="I184" s="42" t="s">
         <v>575</v>
-      </c>
-      <c r="I184" s="42" t="s">
-        <v>576</v>
       </c>
       <c r="J184" s="38" t="s">
         <v>64</v>
@@ -11691,7 +11708,7 @@
         <v>64</v>
       </c>
       <c r="O184" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P184" s="46" t="s">
         <v>64</v>
@@ -11703,7 +11720,7 @@
         <v>228</v>
       </c>
       <c r="S184" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T184" s="38" t="s">
         <v>226</v>
@@ -11731,16 +11748,16 @@
         <v>406</v>
       </c>
       <c r="F185" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G185" s="37" t="s">
         <v>529</v>
       </c>
-      <c r="G185" s="37" t="s">
+      <c r="H185" s="35" t="s">
         <v>530</v>
       </c>
-      <c r="H185" s="35" t="s">
+      <c r="I185" s="42" t="s">
         <v>531</v>
-      </c>
-      <c r="I185" s="42" t="s">
-        <v>532</v>
       </c>
       <c r="J185" s="38" t="s">
         <v>64</v>
@@ -11754,7 +11771,7 @@
         <v>64</v>
       </c>
       <c r="O185" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P185" s="38" t="s">
         <v>64</v>
@@ -11766,7 +11783,7 @@
         <v>228</v>
       </c>
       <c r="S185" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T185" s="38" t="s">
         <v>226</v>
@@ -12016,16 +12033,16 @@
         <v>433</v>
       </c>
       <c r="F192" s="37" t="s">
+        <v>532</v>
+      </c>
+      <c r="G192" s="37" t="s">
         <v>533</v>
       </c>
-      <c r="G192" s="37" t="s">
+      <c r="H192" s="37" t="s">
         <v>534</v>
       </c>
-      <c r="H192" s="37" t="s">
+      <c r="I192" s="42" t="s">
         <v>535</v>
-      </c>
-      <c r="I192" s="42" t="s">
-        <v>536</v>
       </c>
       <c r="J192" s="38" t="s">
         <v>64</v>
@@ -12039,7 +12056,7 @@
         <v>64</v>
       </c>
       <c r="O192" s="38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P192" s="38" t="s">
         <v>64</v>
@@ -12051,7 +12068,7 @@
         <v>228</v>
       </c>
       <c r="S192" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T192" s="38" t="s">
         <v>226</v>
@@ -18370,14 +18387,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b6c6c545-4433-4453-a388-ae81a1a09069" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ae8219d-8505-4e64-b47a-e5e02bd99ff8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18604,15 +18619,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b6c6c545-4433-4453-a388-ae81a1a09069" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ae8219d-8505-4e64-b47a-e5e02bd99ff8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{438C5642-A46B-4670-BCA6-67FA6E6DEAA7}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -18629,18 +18658,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD34699-60E0-49C2-BE80-D215B28F2689}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Adeguamento nuova checklist per INSIEL - CARDIONET - CAW04.04.25
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CARDIONET/CAW04.04.25/accreditamento-checklist_V8.2.6.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CARDIONET/CAW04.04.25/accreditamento-checklist_V8.2.6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\insiel\dati\Divisione Sanità\LB\C@rdionet\ACCREDITAMENTOCDA2\Accreditamento_prima_prova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8297662A-6226-4BCE-8F22-FD89165670DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C656DF1-65E9-4A5D-939B-C5585E92D1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -3102,7 +3102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4252,10 +4252,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="L12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S31" sqref="S31"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5257,7 +5257,7 @@
       <c r="H28" s="37"/>
       <c r="I28" s="42"/>
       <c r="J28" s="38" t="s">
-        <v>228</v>
+        <v>64</v>
       </c>
       <c r="K28" s="38"/>
       <c r="L28" s="38"/>
@@ -5386,7 +5386,7 @@
       <c r="H31" s="37"/>
       <c r="I31" s="42"/>
       <c r="J31" s="38" t="s">
-        <v>228</v>
+        <v>64</v>
       </c>
       <c r="K31" s="38"/>
       <c r="L31" s="38"/>
@@ -18638,7 +18638,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{438C5642-A46B-4670-BCA6-67FA6E6DEAA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45925D79-FB62-4636-8018-56961E1522D0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>